<commit_message>
Investigating political subreddits vs. vparty with reddit_summary.ipynb
</commit_message>
<xml_diff>
--- a/results/vparty/politics.xlsx
+++ b/results/vparty/politics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grace\Desktop\Projects\f20chil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grace\Desktop\Projects\f20chil\results\vparty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{226FFADB-C787-49F2-B8AB-DBE9F5FC7B5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E648E3-B139-45FF-A33F-0D26E08BB145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{045C8682-DDEA-41B1-B881-56EECA593BE3}"/>
   </bookViews>
@@ -1392,19 +1392,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1780,16 +1774,29 @@
   <dimension ref="A1:NT12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="HC15" sqref="HC15"/>
+      <selection activeCell="BC1" sqref="BC1:BE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.7265625" customWidth="1"/>
-    <col min="9" max="9" width="19.08984375" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" customWidth="1"/>
-    <col min="23" max="23" width="8.7265625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="12.54296875" customWidth="1"/>
+    <col min="2" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" hidden="1" customWidth="1"/>
+    <col min="13" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="13.90625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="21.7265625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="18.1796875" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="15.1796875" customWidth="1"/>
+    <col min="27" max="27" width="16.90625" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="0" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="17.26953125" hidden="1" customWidth="1"/>
+    <col min="30" max="53" width="0" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="11.7265625" customWidth="1"/>
+    <col min="55" max="55" width="12.81640625" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="12.90625" hidden="1" customWidth="1"/>
+    <col min="57" max="57" width="13.26953125" hidden="1" customWidth="1"/>
     <col min="210" max="210" width="16" style="2" customWidth="1"/>
     <col min="211" max="211" width="19.26953125" customWidth="1"/>
   </cols>

</xml_diff>